<commit_message>
Excel file was changed
</commit_message>
<xml_diff>
--- a/Mentee-mentor.xlsx
+++ b/Mentee-mentor.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6178" uniqueCount="1452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6177" uniqueCount="1452">
   <si>
     <t>Ф.И.О. ментора</t>
   </si>
@@ -4858,7 +4858,7 @@
   </sheetPr>
   <dimension ref="A1:L1215"/>
   <sheetViews>
-    <sheetView topLeftCell="A1211" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="E1216" sqref="E1216"/>
     </sheetView>
   </sheetViews>
@@ -36863,8 +36863,8 @@
   </sheetPr>
   <dimension ref="A1:I1215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="C233" sqref="C233"/>
+    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -37886,8 +37886,8 @@
       <c r="D38" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>1221</v>
+      <c r="E38" s="4">
+        <v>38</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>34</v>

</xml_diff>